<commit_message>
LRU cache, multithreaded - Working without intermittent crashes
</commit_message>
<xml_diff>
--- a/resources/charts.xlsx
+++ b/resources/charts.xlsx
@@ -94,11 +94,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -127,11 +127,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -153,7 +153,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -166,7 +166,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$4</c:f>
+              <c:f>Sheet1!$A$1:$A$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -187,7 +187,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$4</c:f>
+              <c:f>Sheet1!$B$1:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -216,31 +216,32 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="392133088"/>
-        <c:axId val="390018032"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="392133088"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
+        <c:dropLines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="35000"/>
+                  <a:lumOff val="65000"/>
+                  <a:alpha val="33000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:majorGridlines>
+        </c:dropLines>
+        <c:smooth val="0"/>
+        <c:axId val="179899552"/>
+        <c:axId val="179900672"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="179899552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
         <c:title>
           <c:tx>
             <c:rich>
@@ -250,7 +251,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
+                      <a:schemeClr val="dk1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -283,128 +284,7 @@
               <a:pPr>
                 <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="390018032"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="390018032"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>tuples/s</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
+                    <a:schemeClr val="dk1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -440,6 +320,436 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="179900672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="179900672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tuples/s</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="179899552"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1000"/>
+      </c:valAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Query Latency (10 Ax Finder Queries) vs State Size</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$1:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$1:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2906</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3576</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4867</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5040</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="179902912"/>
+        <c:axId val="179903472"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="179902912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>state size (tuples)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
@@ -455,9 +765,136 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392133088"/>
+        <c:crossAx val="179903472"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="179903472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Query Latency</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="179902912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -473,7 +910,435 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Throughput vs statesize</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F:$F</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G:$G</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1048576"/>
+                <c:pt idx="0">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>402</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>474</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="140714320"/>
+        <c:axId val="140717120"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="140714320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>state size (tuples)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="140717120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="140717120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>tuples</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="140714320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -544,14 +1409,94 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="241">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -563,7 +1508,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -571,7 +1516,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -579,9 +1524,9 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:chartArea mods="allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -594,7 +1539,7 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -609,12 +1554,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -645,33 +1590,47 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="1"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -684,7 +1643,7 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="22225" cap="rnd">
+      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -707,7 +1666,7 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -715,7 +1674,7 @@
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -739,7 +1698,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -747,7 +1706,7 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -772,15 +1731,79 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+            <a:alpha val="33000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -788,17 +1811,35 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
+  </cs:hiLoLine>
+  <cs:leaderLine>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -808,117 +1849,50 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:leaderLine>
   <cs:legend>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -931,7 +1905,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -939,7 +1913,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -959,12 +1933,12 @@
     <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:seriesLine>
@@ -973,12 +1947,12 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1002,35 +1976,72 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="800" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1043,9 +2054,471 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1058,8 +2531,530 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1068,16 +3063,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1091,6 +3086,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1362,44 +3417,132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C4"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J1" activeCellId="1" sqref="K1:K1048576 J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="B1">
+        <v>4000</v>
+      </c>
+      <c r="D1">
+        <v>10000</v>
+      </c>
+      <c r="E1">
+        <v>2906</v>
+      </c>
+      <c r="F1">
+        <v>10000</v>
+      </c>
+      <c r="G1">
+        <v>410</v>
+      </c>
+      <c r="H1">
+        <v>123250</v>
+      </c>
+      <c r="I1">
+        <f>$H1/300</f>
+        <v>410.83333333333331</v>
+      </c>
+      <c r="J1">
+        <v>250</v>
+      </c>
+      <c r="K1">
         <v>4000</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="B2">
         <v>2166</v>
       </c>
+      <c r="D2">
+        <v>100000</v>
+      </c>
+      <c r="E2">
+        <v>3576</v>
+      </c>
+      <c r="F2">
+        <v>100000</v>
+      </c>
+      <c r="G2">
+        <v>496</v>
+      </c>
+      <c r="H2">
+        <v>149000</v>
+      </c>
+      <c r="I2">
+        <f>$H2/300</f>
+        <v>496.66666666666669</v>
+      </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>4</v>
       </c>
-      <c r="C3">
+      <c r="B3">
         <v>2016</v>
       </c>
+      <c r="D3">
+        <v>1000000</v>
+      </c>
+      <c r="E3">
+        <v>4867</v>
+      </c>
+      <c r="F3">
+        <v>1000000</v>
+      </c>
+      <c r="G3">
+        <v>402</v>
+      </c>
+      <c r="H3">
+        <v>120750</v>
+      </c>
+      <c r="I3">
+        <f>$H3/300</f>
+        <v>402.5</v>
+      </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>8</v>
       </c>
-      <c r="C4">
+      <c r="B4">
         <v>2000</v>
+      </c>
+      <c r="D4">
+        <v>10000000</v>
+      </c>
+      <c r="E4">
+        <v>5040</v>
+      </c>
+      <c r="F4">
+        <v>10000000</v>
+      </c>
+      <c r="G4">
+        <v>474</v>
+      </c>
+      <c r="H4">
+        <v>142250</v>
+      </c>
+      <c r="I4">
+        <f>$H4/300</f>
+        <v>474.16666666666669</v>
+      </c>
+    </row>
+    <row r="1048576" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H1048576">
+        <f>SUM(H1:H1048575)</f>
+        <v>535250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tpch Query Implementation - first draft
</commit_message>
<xml_diff>
--- a/resources/charts.xlsx
+++ b/resources/charts.xlsx
@@ -232,11 +232,11 @@
           </c:spPr>
         </c:dropLines>
         <c:smooth val="0"/>
-        <c:axId val="179899552"/>
-        <c:axId val="179900672"/>
+        <c:axId val="174458608"/>
+        <c:axId val="174459728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="179899552"/>
+        <c:axId val="174458608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -335,7 +335,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179900672"/>
+        <c:crossAx val="174459728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -343,7 +343,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="179900672"/>
+        <c:axId val="174459728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -442,7 +442,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179899552"/>
+        <c:crossAx val="174458608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1000"/>
@@ -647,11 +647,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="179902912"/>
-        <c:axId val="179903472"/>
+        <c:axId val="174461968"/>
+        <c:axId val="178731664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="179902912"/>
+        <c:axId val="174461968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -765,12 +765,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179903472"/>
+        <c:crossAx val="178731664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="179903472"/>
+        <c:axId val="178731664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -892,7 +892,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="179902912"/>
+        <c:crossAx val="174461968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1084,11 +1084,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="140714320"/>
-        <c:axId val="140717120"/>
+        <c:axId val="178733904"/>
+        <c:axId val="178734464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="140714320"/>
+        <c:axId val="178733904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1202,12 +1202,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140717120"/>
+        <c:crossAx val="178734464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="140717120"/>
+        <c:axId val="178734464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,7 +1320,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140714320"/>
+        <c:crossAx val="178733904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1332,6 +1332,478 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Throughput Comparision:</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Aggregate() Vs partitionPersist() + Drpc </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>DRPC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Aggregation</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="338773744"/>
+        <c:axId val="338773184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="338773744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Drpc State Queries are Expensive</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="@" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="338773184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="338773184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>tuples</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="338773744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17077799650043743"/>
+          <c:y val="0.83854111986001745"/>
+          <c:w val="0.75844400699912518"/>
+          <c:h val="7.8125546806649182E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1489,6 +1961,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
   <cs:axisTitle>
@@ -3040,6 +3552,500 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3146,6 +4152,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3419,8 +4455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" activeCellId="1" sqref="K1:K1048576 J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J1" activeCellId="1" sqref="K1 J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>